<commit_message>
LAND USE O CARALHO
</commit_message>
<xml_diff>
--- a/cos/dominant.xlsx
+++ b/cos/dominant.xlsx
@@ -774,7 +774,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -799,7 +799,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -849,7 +849,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1424,7 +1424,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3024,7 +3024,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D104" t="n">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D105" t="n">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D110" t="n">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3574,7 +3574,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -3624,7 +3624,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3999,7 +3999,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -4024,7 +4024,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D145" t="n">
@@ -4074,7 +4074,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D147" t="n">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D148" t="n">
@@ -4149,7 +4149,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4174,7 +4174,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D152" t="n">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4474,7 +4474,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4499,7 +4499,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4524,7 +4524,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -4774,7 +4774,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -4799,7 +4799,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D175" t="n">
@@ -4824,7 +4824,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -4874,7 +4874,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -4899,7 +4899,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Urbanizado</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D181" t="n">

</xml_diff>

<commit_message>
override transporte buffer = 75 metros, + nº de ocurrências por classe + média por classe
</commit_message>
<xml_diff>
--- a/cos/dominant.xlsx
+++ b/cos/dominant.xlsx
@@ -2274,7 +2274,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D110" t="n">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -4074,7 +4074,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D147" t="n">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D148" t="n">
@@ -4149,7 +4149,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4174,7 +4174,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D152" t="n">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4774,7 +4774,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -4799,7 +4799,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D175" t="n">
@@ -4824,7 +4824,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -4874,7 +4874,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -4899,7 +4899,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Urbanizado</t>
         </is>
       </c>
       <c r="D181" t="n">

</xml_diff>